<commit_message>
Protection to workspaces and jin Tab addes
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\ScoutsWallet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1B36087-9D3C-49D4-922F-C09BA048E7F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFA83AB4-FF43-4FF6-9DCA-0136004267AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -91,7 +91,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -144,17 +144,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -169,25 +158,92 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -495,8 +551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -504,666 +560,667 @@
     <col min="1" max="1" width="44.5703125" customWidth="1"/>
     <col min="2" max="2" width="28.5703125" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="44.5703125" customWidth="1"/>
-    <col min="5" max="5" width="40.7109375" customWidth="1"/>
-    <col min="6" max="6" width="43.28515625" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" customWidth="1"/>
+    <col min="4" max="4" width="44.5703125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="40.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="43.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="14.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="D2" s="3"/>
+      <c r="B2" s="8"/>
+      <c r="D2" s="9"/>
       <c r="F2" s="3"/>
     </row>
     <row r="3" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="4"/>
-      <c r="D3" s="3"/>
+      <c r="A3" s="10"/>
+      <c r="B3" s="8"/>
+      <c r="D3" s="9"/>
     </row>
     <row r="4" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="4"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="8"/>
     </row>
     <row r="5" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="4"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="8"/>
     </row>
     <row r="6" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="4"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="8"/>
     </row>
     <row r="7" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="4"/>
+      <c r="A7" s="10"/>
+      <c r="B7" s="8"/>
     </row>
     <row r="8" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="4"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="8"/>
     </row>
     <row r="9" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="4"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="8"/>
     </row>
     <row r="10" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="4"/>
+      <c r="A10" s="10"/>
+      <c r="B10" s="8"/>
     </row>
     <row r="11" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="4"/>
+      <c r="A11" s="10"/>
+      <c r="B11" s="8"/>
     </row>
     <row r="12" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
-      <c r="B12" s="4"/>
+      <c r="A12" s="11"/>
+      <c r="B12" s="8"/>
     </row>
     <row r="13" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
-      <c r="B13" s="4"/>
-      <c r="D13" s="6" t="s">
+      <c r="A13" s="12"/>
+      <c r="B13" s="8"/>
+      <c r="D13" s="13" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="4"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="8">
+      <c r="B14" s="8"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="15">
         <f>SUM(B:B)</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="4"/>
+      <c r="B15" s="8"/>
     </row>
     <row r="16" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="4"/>
+      <c r="B16" s="8"/>
     </row>
     <row r="17" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="4"/>
+      <c r="B17" s="8"/>
     </row>
     <row r="18" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="4"/>
+      <c r="B18" s="8"/>
     </row>
     <row r="19" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="4"/>
+      <c r="B19" s="8"/>
     </row>
     <row r="20" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="4"/>
+      <c r="B20" s="8"/>
     </row>
     <row r="21" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="4"/>
+      <c r="B21" s="8"/>
     </row>
     <row r="22" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="4"/>
+      <c r="B22" s="8"/>
     </row>
     <row r="23" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="4"/>
+      <c r="B23" s="8"/>
     </row>
     <row r="24" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="4"/>
+      <c r="B24" s="8"/>
     </row>
     <row r="25" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="4"/>
+      <c r="B25" s="8"/>
     </row>
     <row r="26" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="4"/>
+      <c r="B26" s="8"/>
     </row>
     <row r="27" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="4"/>
+      <c r="B27" s="8"/>
     </row>
     <row r="28" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="4"/>
+      <c r="B28" s="8"/>
     </row>
     <row r="29" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="4"/>
+      <c r="B29" s="8"/>
     </row>
     <row r="30" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="4"/>
+      <c r="B30" s="8"/>
     </row>
     <row r="31" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="4"/>
+      <c r="B31" s="8"/>
     </row>
     <row r="32" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="4"/>
+      <c r="B32" s="8"/>
     </row>
     <row r="33" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="4"/>
+      <c r="B33" s="8"/>
     </row>
     <row r="34" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="4"/>
+      <c r="B34" s="8"/>
     </row>
     <row r="35" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="4"/>
+      <c r="B35" s="8"/>
     </row>
     <row r="36" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="4"/>
+      <c r="B36" s="8"/>
     </row>
     <row r="37" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="4"/>
+      <c r="B37" s="8"/>
     </row>
     <row r="38" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="4"/>
+      <c r="B38" s="8"/>
     </row>
     <row r="39" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="4"/>
+      <c r="B39" s="8"/>
     </row>
     <row r="40" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="4"/>
+      <c r="B40" s="8"/>
     </row>
     <row r="41" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="4"/>
+      <c r="B41" s="8"/>
     </row>
     <row r="42" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="4"/>
+      <c r="B42" s="8"/>
     </row>
     <row r="43" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="4"/>
+      <c r="B43" s="8"/>
     </row>
     <row r="44" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="4"/>
+      <c r="B44" s="8"/>
     </row>
     <row r="45" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="4"/>
+      <c r="B45" s="8"/>
     </row>
     <row r="46" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="4"/>
+      <c r="B46" s="8"/>
     </row>
     <row r="47" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="4"/>
+      <c r="B47" s="8"/>
     </row>
     <row r="48" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="4"/>
+      <c r="B48" s="8"/>
     </row>
     <row r="49" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="4"/>
+      <c r="B49" s="8"/>
     </row>
     <row r="50" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="4"/>
+      <c r="B50" s="8"/>
     </row>
     <row r="51" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="4"/>
+      <c r="B51" s="8"/>
     </row>
     <row r="52" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="4"/>
+      <c r="B52" s="8"/>
     </row>
     <row r="53" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="4"/>
+      <c r="B53" s="8"/>
     </row>
     <row r="54" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="4"/>
+      <c r="B54" s="8"/>
     </row>
     <row r="55" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="4"/>
+      <c r="B55" s="8"/>
     </row>
     <row r="56" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="4"/>
+      <c r="B56" s="8"/>
     </row>
     <row r="57" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="4"/>
+      <c r="B57" s="8"/>
     </row>
     <row r="58" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="4"/>
+      <c r="B58" s="8"/>
     </row>
     <row r="59" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="4"/>
+      <c r="B59" s="8"/>
     </row>
     <row r="60" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="4"/>
+      <c r="B60" s="8"/>
     </row>
     <row r="61" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="4"/>
+      <c r="B61" s="8"/>
     </row>
     <row r="62" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="4"/>
+      <c r="B62" s="8"/>
     </row>
     <row r="63" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="4"/>
+      <c r="B63" s="8"/>
     </row>
     <row r="64" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="4"/>
+      <c r="B64" s="8"/>
     </row>
     <row r="65" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="4"/>
+      <c r="B65" s="8"/>
     </row>
     <row r="66" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="4"/>
+      <c r="B66" s="8"/>
     </row>
     <row r="67" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="4"/>
+      <c r="B67" s="8"/>
     </row>
     <row r="68" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="4"/>
+      <c r="B68" s="8"/>
     </row>
     <row r="69" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="4"/>
+      <c r="B69" s="8"/>
     </row>
     <row r="70" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="4"/>
+      <c r="B70" s="8"/>
     </row>
     <row r="71" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="4"/>
+      <c r="B71" s="8"/>
     </row>
     <row r="72" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="4"/>
+      <c r="B72" s="8"/>
     </row>
     <row r="73" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="4"/>
+      <c r="B73" s="8"/>
     </row>
     <row r="74" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="4"/>
+      <c r="B74" s="8"/>
     </row>
     <row r="75" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="4"/>
+      <c r="B75" s="8"/>
     </row>
     <row r="76" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="4"/>
+      <c r="B76" s="8"/>
     </row>
     <row r="77" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="4"/>
+      <c r="B77" s="8"/>
     </row>
     <row r="78" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B78" s="4"/>
+      <c r="B78" s="8"/>
     </row>
     <row r="79" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="4"/>
+      <c r="B79" s="8"/>
     </row>
     <row r="80" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B80" s="4"/>
+      <c r="B80" s="8"/>
     </row>
     <row r="81" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B81" s="4"/>
+      <c r="B81" s="8"/>
     </row>
     <row r="82" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B82" s="4"/>
+      <c r="B82" s="8"/>
     </row>
     <row r="83" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="4"/>
+      <c r="B83" s="8"/>
     </row>
     <row r="84" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B84" s="4"/>
+      <c r="B84" s="8"/>
     </row>
     <row r="85" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B85" s="4"/>
+      <c r="B85" s="8"/>
     </row>
     <row r="86" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B86" s="4"/>
+      <c r="B86" s="8"/>
     </row>
     <row r="87" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B87" s="4"/>
+      <c r="B87" s="8"/>
     </row>
     <row r="88" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B88" s="4"/>
+      <c r="B88" s="8"/>
     </row>
     <row r="89" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B89" s="4"/>
+      <c r="B89" s="8"/>
     </row>
     <row r="90" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B90" s="4"/>
+      <c r="B90" s="8"/>
     </row>
     <row r="91" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B91" s="4"/>
+      <c r="B91" s="8"/>
     </row>
     <row r="92" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B92" s="4"/>
+      <c r="B92" s="8"/>
     </row>
     <row r="93" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B93" s="4"/>
+      <c r="B93" s="8"/>
     </row>
     <row r="94" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B94" s="4"/>
+      <c r="B94" s="8"/>
     </row>
     <row r="95" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B95" s="4"/>
+      <c r="B95" s="8"/>
     </row>
     <row r="96" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B96" s="4"/>
+      <c r="B96" s="8"/>
     </row>
     <row r="97" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B97" s="4"/>
+      <c r="B97" s="8"/>
     </row>
     <row r="98" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B98" s="4"/>
+      <c r="B98" s="8"/>
     </row>
     <row r="99" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B99" s="4"/>
+      <c r="B99" s="8"/>
     </row>
     <row r="100" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B100" s="4"/>
+      <c r="B100" s="8"/>
     </row>
     <row r="101" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B101" s="4"/>
+      <c r="B101" s="8"/>
     </row>
     <row r="102" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B102" s="4"/>
+      <c r="B102" s="8"/>
     </row>
     <row r="103" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B103" s="4"/>
+      <c r="B103" s="8"/>
     </row>
     <row r="104" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B104" s="4"/>
+      <c r="B104" s="8"/>
     </row>
     <row r="105" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B105" s="4"/>
+      <c r="B105" s="8"/>
     </row>
     <row r="106" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B106" s="4"/>
+      <c r="B106" s="8"/>
     </row>
     <row r="107" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B107" s="4"/>
+      <c r="B107" s="8"/>
     </row>
     <row r="108" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B108" s="4"/>
+      <c r="B108" s="8"/>
     </row>
     <row r="109" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B109" s="4"/>
+      <c r="B109" s="8"/>
     </row>
     <row r="110" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B110" s="4"/>
+      <c r="B110" s="8"/>
     </row>
     <row r="111" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B111" s="4"/>
+      <c r="B111" s="8"/>
     </row>
     <row r="112" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B112" s="4"/>
+      <c r="B112" s="8"/>
     </row>
     <row r="113" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B113" s="4"/>
+      <c r="B113" s="8"/>
     </row>
     <row r="114" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B114" s="4"/>
+      <c r="B114" s="8"/>
     </row>
     <row r="115" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B115" s="4"/>
+      <c r="B115" s="8"/>
     </row>
     <row r="116" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B116" s="4"/>
+      <c r="B116" s="8"/>
     </row>
     <row r="117" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B117" s="4"/>
+      <c r="B117" s="8"/>
     </row>
     <row r="118" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B118" s="4"/>
+      <c r="B118" s="8"/>
     </row>
     <row r="119" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B119" s="4"/>
+      <c r="B119" s="8"/>
     </row>
     <row r="120" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B120" s="4"/>
+      <c r="B120" s="8"/>
     </row>
     <row r="121" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B121" s="4"/>
+      <c r="B121" s="8"/>
     </row>
     <row r="122" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B122" s="4"/>
+      <c r="B122" s="8"/>
     </row>
     <row r="123" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B123" s="4"/>
+      <c r="B123" s="8"/>
     </row>
     <row r="124" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B124" s="4"/>
+      <c r="B124" s="8"/>
     </row>
     <row r="125" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B125" s="4"/>
+      <c r="B125" s="8"/>
     </row>
     <row r="126" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B126" s="4"/>
+      <c r="B126" s="8"/>
     </row>
     <row r="127" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B127" s="4"/>
+      <c r="B127" s="8"/>
     </row>
     <row r="128" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B128" s="4"/>
+      <c r="B128" s="8"/>
     </row>
     <row r="129" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B129" s="4"/>
+      <c r="B129" s="8"/>
     </row>
     <row r="130" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B130" s="4"/>
+      <c r="B130" s="8"/>
     </row>
     <row r="131" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B131" s="4"/>
+      <c r="B131" s="8"/>
     </row>
     <row r="132" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B132" s="4"/>
+      <c r="B132" s="8"/>
     </row>
     <row r="133" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B133" s="4"/>
+      <c r="B133" s="8"/>
     </row>
     <row r="134" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B134" s="4"/>
+      <c r="B134" s="8"/>
     </row>
     <row r="135" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B135" s="4"/>
+      <c r="B135" s="8"/>
     </row>
     <row r="136" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B136" s="4"/>
+      <c r="B136" s="8"/>
     </row>
     <row r="137" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B137" s="4"/>
+      <c r="B137" s="8"/>
     </row>
     <row r="138" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B138" s="4"/>
+      <c r="B138" s="8"/>
     </row>
     <row r="139" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B139" s="4"/>
+      <c r="B139" s="8"/>
     </row>
     <row r="140" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B140" s="4"/>
+      <c r="B140" s="8"/>
     </row>
     <row r="141" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B141" s="4"/>
+      <c r="B141" s="8"/>
     </row>
     <row r="142" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B142" s="4"/>
+      <c r="B142" s="8"/>
     </row>
     <row r="143" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B143" s="4"/>
+      <c r="B143" s="8"/>
     </row>
     <row r="144" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B144" s="4"/>
+      <c r="B144" s="8"/>
     </row>
     <row r="145" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B145" s="4"/>
+      <c r="B145" s="8"/>
     </row>
     <row r="146" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B146" s="4"/>
+      <c r="B146" s="8"/>
     </row>
     <row r="147" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B147" s="4"/>
+      <c r="B147" s="8"/>
     </row>
     <row r="148" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B148" s="4"/>
+      <c r="B148" s="8"/>
     </row>
     <row r="149" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B149" s="4"/>
+      <c r="B149" s="8"/>
     </row>
     <row r="150" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B150" s="4"/>
+      <c r="B150" s="8"/>
     </row>
     <row r="151" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B151" s="4"/>
+      <c r="B151" s="8"/>
     </row>
     <row r="152" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B152" s="4"/>
+      <c r="B152" s="8"/>
     </row>
     <row r="153" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B153" s="4"/>
+      <c r="B153" s="8"/>
     </row>
     <row r="154" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B154" s="4"/>
+      <c r="B154" s="8"/>
     </row>
     <row r="155" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B155" s="4"/>
+      <c r="B155" s="8"/>
     </row>
     <row r="156" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B156" s="4"/>
+      <c r="B156" s="8"/>
     </row>
     <row r="157" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B157" s="4"/>
+      <c r="B157" s="8"/>
     </row>
     <row r="158" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B158" s="4"/>
+      <c r="B158" s="8"/>
     </row>
     <row r="159" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B159" s="4"/>
+      <c r="B159" s="8"/>
     </row>
     <row r="160" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B160" s="4"/>
+      <c r="B160" s="8"/>
     </row>
     <row r="161" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B161" s="4"/>
+      <c r="B161" s="8"/>
     </row>
     <row r="162" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B162" s="4"/>
+      <c r="B162" s="8"/>
     </row>
     <row r="163" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B163" s="4"/>
+      <c r="B163" s="8"/>
     </row>
     <row r="164" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B164" s="4"/>
+      <c r="B164" s="8"/>
     </row>
     <row r="165" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B165" s="4"/>
+      <c r="B165" s="8"/>
     </row>
     <row r="166" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B166" s="4"/>
+      <c r="B166" s="8"/>
     </row>
     <row r="167" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B167" s="4"/>
+      <c r="B167" s="8"/>
     </row>
     <row r="168" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B168" s="4"/>
+      <c r="B168" s="8"/>
     </row>
     <row r="169" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B169" s="4"/>
+      <c r="B169" s="8"/>
     </row>
     <row r="170" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B170" s="4"/>
+      <c r="B170" s="8"/>
     </row>
     <row r="171" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B171" s="4"/>
+      <c r="B171" s="8"/>
     </row>
     <row r="172" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B172" s="4"/>
+      <c r="B172" s="8"/>
     </row>
     <row r="173" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B173" s="4"/>
+      <c r="B173" s="8"/>
     </row>
     <row r="174" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B174" s="4"/>
+      <c r="B174" s="8"/>
     </row>
     <row r="175" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B175" s="4"/>
+      <c r="B175" s="8"/>
     </row>
     <row r="176" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B176" s="4"/>
+      <c r="B176" s="8"/>
     </row>
     <row r="177" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B177" s="4"/>
+      <c r="B177" s="8"/>
     </row>
     <row r="178" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B178" s="4"/>
+      <c r="B178" s="8"/>
     </row>
     <row r="179" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B179" s="4"/>
+      <c r="B179" s="8"/>
     </row>
     <row r="180" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B180" s="4"/>
+      <c r="B180" s="8"/>
     </row>
     <row r="181" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B181" s="4"/>
+      <c r="B181" s="8"/>
     </row>
     <row r="182" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B182" s="4"/>
+      <c r="B182" s="8"/>
     </row>
     <row r="183" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B183" s="4"/>
+      <c r="B183" s="8"/>
     </row>
     <row r="184" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B184" s="4"/>
+      <c r="B184" s="8"/>
     </row>
     <row r="185" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B185" s="4"/>
+      <c r="B185" s="8"/>
     </row>
     <row r="186" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B186" s="4"/>
+      <c r="B186" s="8"/>
     </row>
     <row r="187" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B187" s="4"/>
+      <c r="B187" s="8"/>
     </row>
     <row r="188" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B188" s="4"/>
+      <c r="B188" s="8"/>
     </row>
     <row r="189" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B189" s="4"/>
+      <c r="B189" s="8"/>
     </row>
     <row r="190" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B190" s="4"/>
+      <c r="B190" s="8"/>
     </row>
     <row r="191" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B191" s="4"/>
+      <c r="B191" s="8"/>
     </row>
     <row r="192" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B192" s="4"/>
+      <c r="B192" s="8"/>
     </row>
     <row r="193" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B193" s="4"/>
+      <c r="B193" s="8"/>
     </row>
     <row r="194" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B194" s="4"/>
+      <c r="B194" s="8"/>
     </row>
     <row r="195" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B195" s="4"/>
+      <c r="B195" s="8"/>
     </row>
     <row r="196" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B196" s="4"/>
+      <c r="B196" s="8"/>
     </row>
     <row r="197" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B197" s="4"/>
+      <c r="B197" s="8"/>
     </row>
     <row r="198" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B198" s="4"/>
+      <c r="B198" s="8"/>
     </row>
     <row r="199" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B199" s="4"/>
+      <c r="B199" s="8"/>
     </row>
     <row r="200" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B200" s="4"/>
+      <c r="B200" s="8"/>
     </row>
     <row r="201" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B201" s="4"/>
+      <c r="B201" s="8"/>
     </row>
     <row r="202" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B202" s="4"/>
+      <c r="B202" s="8"/>
     </row>
     <row r="203" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B203" s="4"/>
+      <c r="B203" s="8"/>
     </row>
     <row r="204" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B204" s="4"/>
+      <c r="B204" s="8"/>
     </row>
     <row r="205" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B205" s="4"/>
+      <c r="B205" s="8"/>
     </row>
     <row r="206" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B206" s="4"/>
+      <c r="B206" s="8"/>
     </row>
     <row r="207" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B207" s="4"/>
+      <c r="B207" s="8"/>
     </row>
     <row r="208" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B208" s="4"/>
+      <c r="B208" s="8"/>
     </row>
     <row r="209" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="210" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1958,6 +2015,7 @@
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="k9AlNkVvuNBN+E6gqZZZM8rNcVP/1VXMgFgB6HYsJ97tR7Xub9SbT53XqzsE2xACJRTqCTwbk7y1I58/9n6vfw==" saltValue="qFIVyIQYqjLzjNphOGA9NQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <conditionalFormatting sqref="B2:B988">
     <cfRule type="cellIs" dxfId="7" priority="1" operator="lessThan">
       <formula>0</formula>
@@ -1984,7 +2042,7 @@
   <dimension ref="A1:I1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1993,692 +2051,693 @@
     <col min="2" max="2" width="28.5703125" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
     <col min="4" max="4" width="36.42578125" customWidth="1"/>
-    <col min="5" max="5" width="22.28515625" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" style="18" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="14.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="4"/>
+      <c r="B2" s="8"/>
     </row>
     <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="4"/>
-      <c r="D3" s="1" t="s">
+      <c r="B3" s="8"/>
+      <c r="D3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="19">
         <f>SUM((B:B))</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="4"/>
-      <c r="D4" s="6" t="s">
+      <c r="B4" s="8"/>
+      <c r="D4" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="9"/>
+      <c r="E4" s="20"/>
     </row>
     <row r="5" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="4"/>
-      <c r="D5" s="12" t="s">
+      <c r="B5" s="8"/>
+      <c r="D5" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="9"/>
+      <c r="E5" s="20"/>
     </row>
     <row r="6" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="4"/>
+      <c r="B6" s="8"/>
     </row>
     <row r="7" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="4"/>
+      <c r="B7" s="8"/>
     </row>
     <row r="8" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="4"/>
+      <c r="B8" s="8"/>
     </row>
     <row r="9" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="4"/>
+      <c r="B9" s="8"/>
     </row>
     <row r="10" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="4"/>
+      <c r="B10" s="8"/>
     </row>
     <row r="11" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="4"/>
+      <c r="B11" s="8"/>
     </row>
     <row r="12" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="4"/>
+      <c r="B12" s="8"/>
     </row>
     <row r="13" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="4"/>
+      <c r="B13" s="8"/>
     </row>
     <row r="14" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="4"/>
+      <c r="B14" s="8"/>
     </row>
     <row r="15" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="4"/>
+      <c r="B15" s="8"/>
     </row>
     <row r="16" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="4"/>
+      <c r="B16" s="8"/>
     </row>
     <row r="17" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="4"/>
+      <c r="B17" s="8"/>
     </row>
     <row r="18" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="4"/>
+      <c r="B18" s="8"/>
     </row>
     <row r="19" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="4"/>
+      <c r="B19" s="8"/>
     </row>
     <row r="20" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="4"/>
+      <c r="B20" s="8"/>
     </row>
     <row r="21" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="4"/>
+      <c r="B21" s="8"/>
     </row>
     <row r="22" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="4"/>
+      <c r="B22" s="8"/>
     </row>
     <row r="23" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="4"/>
+      <c r="B23" s="8"/>
     </row>
     <row r="24" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="4"/>
+      <c r="B24" s="8"/>
     </row>
     <row r="25" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="4"/>
+      <c r="B25" s="8"/>
     </row>
     <row r="26" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="4"/>
+      <c r="B26" s="8"/>
     </row>
     <row r="27" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="4"/>
+      <c r="B27" s="8"/>
     </row>
     <row r="28" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="4"/>
+      <c r="B28" s="8"/>
     </row>
     <row r="29" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="4"/>
+      <c r="B29" s="8"/>
     </row>
     <row r="30" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="4"/>
+      <c r="B30" s="8"/>
     </row>
     <row r="31" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="4"/>
+      <c r="B31" s="8"/>
     </row>
     <row r="32" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="4"/>
-      <c r="I32" t="s">
+      <c r="B32" s="8"/>
+      <c r="I32" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="33" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="4"/>
+      <c r="B33" s="8"/>
     </row>
     <row r="34" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="4"/>
+      <c r="B34" s="8"/>
     </row>
     <row r="35" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="4"/>
+      <c r="B35" s="8"/>
     </row>
     <row r="36" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="4"/>
+      <c r="B36" s="8"/>
     </row>
     <row r="37" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="4"/>
+      <c r="B37" s="8"/>
     </row>
     <row r="38" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="4"/>
+      <c r="B38" s="8"/>
     </row>
     <row r="39" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="4"/>
+      <c r="B39" s="8"/>
     </row>
     <row r="40" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="4"/>
+      <c r="B40" s="8"/>
     </row>
     <row r="41" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="4"/>
+      <c r="B41" s="8"/>
     </row>
     <row r="42" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="4"/>
+      <c r="B42" s="8"/>
     </row>
     <row r="43" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="4"/>
+      <c r="B43" s="8"/>
     </row>
     <row r="44" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="4"/>
+      <c r="B44" s="8"/>
     </row>
     <row r="45" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="4"/>
+      <c r="B45" s="8"/>
     </row>
     <row r="46" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="4"/>
+      <c r="B46" s="8"/>
     </row>
     <row r="47" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="4"/>
+      <c r="B47" s="8"/>
     </row>
     <row r="48" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="4"/>
+      <c r="B48" s="8"/>
     </row>
     <row r="49" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="4"/>
+      <c r="B49" s="8"/>
     </row>
     <row r="50" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="4"/>
+      <c r="B50" s="8"/>
     </row>
     <row r="51" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="4"/>
+      <c r="B51" s="8"/>
     </row>
     <row r="52" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="4"/>
+      <c r="B52" s="8"/>
     </row>
     <row r="53" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="4"/>
+      <c r="B53" s="8"/>
     </row>
     <row r="54" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="4"/>
+      <c r="B54" s="8"/>
     </row>
     <row r="55" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="4"/>
+      <c r="B55" s="8"/>
     </row>
     <row r="56" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="4"/>
+      <c r="B56" s="8"/>
     </row>
     <row r="57" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="4"/>
+      <c r="B57" s="8"/>
     </row>
     <row r="58" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="4"/>
+      <c r="B58" s="8"/>
     </row>
     <row r="59" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="4"/>
+      <c r="B59" s="8"/>
     </row>
     <row r="60" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="4"/>
+      <c r="B60" s="8"/>
     </row>
     <row r="61" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="4"/>
+      <c r="B61" s="8"/>
     </row>
     <row r="62" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="4"/>
+      <c r="B62" s="8"/>
     </row>
     <row r="63" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="4"/>
+      <c r="B63" s="8"/>
     </row>
     <row r="64" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="4"/>
+      <c r="B64" s="8"/>
     </row>
     <row r="65" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="4"/>
+      <c r="B65" s="8"/>
     </row>
     <row r="66" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="4"/>
+      <c r="B66" s="8"/>
     </row>
     <row r="67" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="4"/>
+      <c r="B67" s="8"/>
     </row>
     <row r="68" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="4"/>
+      <c r="B68" s="8"/>
     </row>
     <row r="69" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="4"/>
+      <c r="B69" s="8"/>
     </row>
     <row r="70" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="4"/>
+      <c r="B70" s="8"/>
     </row>
     <row r="71" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="4"/>
+      <c r="B71" s="8"/>
     </row>
     <row r="72" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="4"/>
+      <c r="B72" s="8"/>
     </row>
     <row r="73" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="4"/>
+      <c r="B73" s="8"/>
     </row>
     <row r="74" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="4"/>
+      <c r="B74" s="8"/>
     </row>
     <row r="75" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="4"/>
+      <c r="B75" s="8"/>
     </row>
     <row r="76" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="4"/>
+      <c r="B76" s="8"/>
     </row>
     <row r="77" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="4"/>
+      <c r="B77" s="8"/>
     </row>
     <row r="78" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B78" s="4"/>
+      <c r="B78" s="8"/>
     </row>
     <row r="79" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="4"/>
+      <c r="B79" s="8"/>
     </row>
     <row r="80" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B80" s="4"/>
+      <c r="B80" s="8"/>
     </row>
     <row r="81" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B81" s="4"/>
+      <c r="B81" s="8"/>
     </row>
     <row r="82" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B82" s="4"/>
+      <c r="B82" s="8"/>
     </row>
     <row r="83" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="4"/>
+      <c r="B83" s="8"/>
     </row>
     <row r="84" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B84" s="4"/>
+      <c r="B84" s="8"/>
     </row>
     <row r="85" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B85" s="4"/>
+      <c r="B85" s="8"/>
     </row>
     <row r="86" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B86" s="4"/>
+      <c r="B86" s="8"/>
     </row>
     <row r="87" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B87" s="4"/>
+      <c r="B87" s="8"/>
     </row>
     <row r="88" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B88" s="4"/>
+      <c r="B88" s="8"/>
     </row>
     <row r="89" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B89" s="4"/>
+      <c r="B89" s="8"/>
     </row>
     <row r="90" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B90" s="4"/>
+      <c r="B90" s="8"/>
     </row>
     <row r="91" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B91" s="4"/>
+      <c r="B91" s="8"/>
     </row>
     <row r="92" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B92" s="4"/>
+      <c r="B92" s="8"/>
     </row>
     <row r="93" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B93" s="4"/>
+      <c r="B93" s="8"/>
     </row>
     <row r="94" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B94" s="4"/>
+      <c r="B94" s="8"/>
     </row>
     <row r="95" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B95" s="4"/>
+      <c r="B95" s="8"/>
     </row>
     <row r="96" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B96" s="4"/>
+      <c r="B96" s="8"/>
     </row>
     <row r="97" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B97" s="4"/>
+      <c r="B97" s="8"/>
     </row>
     <row r="98" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B98" s="4"/>
+      <c r="B98" s="8"/>
     </row>
     <row r="99" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B99" s="4"/>
+      <c r="B99" s="8"/>
     </row>
     <row r="100" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B100" s="4"/>
+      <c r="B100" s="8"/>
     </row>
     <row r="101" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B101" s="4"/>
+      <c r="B101" s="8"/>
     </row>
     <row r="102" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B102" s="4"/>
+      <c r="B102" s="8"/>
     </row>
     <row r="103" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B103" s="4"/>
+      <c r="B103" s="8"/>
     </row>
     <row r="104" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B104" s="4"/>
+      <c r="B104" s="8"/>
     </row>
     <row r="105" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B105" s="4"/>
+      <c r="B105" s="8"/>
     </row>
     <row r="106" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B106" s="4"/>
+      <c r="B106" s="8"/>
     </row>
     <row r="107" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B107" s="4"/>
+      <c r="B107" s="8"/>
     </row>
     <row r="108" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B108" s="4"/>
+      <c r="B108" s="8"/>
     </row>
     <row r="109" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B109" s="4"/>
+      <c r="B109" s="8"/>
     </row>
     <row r="110" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B110" s="4"/>
+      <c r="B110" s="8"/>
     </row>
     <row r="111" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B111" s="4"/>
+      <c r="B111" s="8"/>
     </row>
     <row r="112" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B112" s="4"/>
+      <c r="B112" s="8"/>
     </row>
     <row r="113" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B113" s="4"/>
+      <c r="B113" s="8"/>
     </row>
     <row r="114" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B114" s="4"/>
+      <c r="B114" s="8"/>
     </row>
     <row r="115" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B115" s="4"/>
+      <c r="B115" s="8"/>
     </row>
     <row r="116" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B116" s="4"/>
+      <c r="B116" s="8"/>
     </row>
     <row r="117" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B117" s="4"/>
+      <c r="B117" s="8"/>
     </row>
     <row r="118" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B118" s="4"/>
+      <c r="B118" s="8"/>
     </row>
     <row r="119" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B119" s="4"/>
+      <c r="B119" s="8"/>
     </row>
     <row r="120" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B120" s="4"/>
+      <c r="B120" s="8"/>
     </row>
     <row r="121" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B121" s="4"/>
+      <c r="B121" s="8"/>
     </row>
     <row r="122" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B122" s="4"/>
+      <c r="B122" s="8"/>
     </row>
     <row r="123" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B123" s="4"/>
+      <c r="B123" s="8"/>
     </row>
     <row r="124" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B124" s="4"/>
+      <c r="B124" s="8"/>
     </row>
     <row r="125" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B125" s="4"/>
+      <c r="B125" s="8"/>
     </row>
     <row r="126" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B126" s="4"/>
+      <c r="B126" s="8"/>
     </row>
     <row r="127" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B127" s="4"/>
+      <c r="B127" s="8"/>
     </row>
     <row r="128" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B128" s="4"/>
+      <c r="B128" s="8"/>
     </row>
     <row r="129" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B129" s="4"/>
+      <c r="B129" s="8"/>
     </row>
     <row r="130" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B130" s="4"/>
+      <c r="B130" s="8"/>
     </row>
     <row r="131" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B131" s="4"/>
+      <c r="B131" s="8"/>
     </row>
     <row r="132" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B132" s="4"/>
+      <c r="B132" s="8"/>
     </row>
     <row r="133" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B133" s="4"/>
+      <c r="B133" s="8"/>
     </row>
     <row r="134" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B134" s="4"/>
+      <c r="B134" s="8"/>
     </row>
     <row r="135" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B135" s="4"/>
+      <c r="B135" s="8"/>
     </row>
     <row r="136" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B136" s="4"/>
+      <c r="B136" s="8"/>
     </row>
     <row r="137" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B137" s="4"/>
+      <c r="B137" s="8"/>
     </row>
     <row r="138" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B138" s="4"/>
+      <c r="B138" s="8"/>
     </row>
     <row r="139" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B139" s="4"/>
+      <c r="B139" s="8"/>
     </row>
     <row r="140" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B140" s="4"/>
+      <c r="B140" s="8"/>
     </row>
     <row r="141" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B141" s="4"/>
+      <c r="B141" s="8"/>
     </row>
     <row r="142" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B142" s="4"/>
+      <c r="B142" s="8"/>
     </row>
     <row r="143" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B143" s="4"/>
+      <c r="B143" s="8"/>
     </row>
     <row r="144" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B144" s="4"/>
+      <c r="B144" s="8"/>
     </row>
     <row r="145" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B145" s="4"/>
+      <c r="B145" s="8"/>
     </row>
     <row r="146" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B146" s="4"/>
+      <c r="B146" s="8"/>
     </row>
     <row r="147" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B147" s="4"/>
+      <c r="B147" s="8"/>
     </row>
     <row r="148" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B148" s="4"/>
+      <c r="B148" s="8"/>
     </row>
     <row r="149" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B149" s="4"/>
+      <c r="B149" s="8"/>
     </row>
     <row r="150" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B150" s="4"/>
+      <c r="B150" s="8"/>
     </row>
     <row r="151" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B151" s="4"/>
+      <c r="B151" s="8"/>
     </row>
     <row r="152" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B152" s="4"/>
+      <c r="B152" s="8"/>
     </row>
     <row r="153" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B153" s="4"/>
+      <c r="B153" s="8"/>
     </row>
     <row r="154" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B154" s="4"/>
+      <c r="B154" s="8"/>
     </row>
     <row r="155" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B155" s="4"/>
+      <c r="B155" s="8"/>
     </row>
     <row r="156" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B156" s="4"/>
+      <c r="B156" s="8"/>
     </row>
     <row r="157" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B157" s="4"/>
+      <c r="B157" s="8"/>
     </row>
     <row r="158" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B158" s="4"/>
+      <c r="B158" s="8"/>
     </row>
     <row r="159" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B159" s="4"/>
+      <c r="B159" s="8"/>
     </row>
     <row r="160" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B160" s="4"/>
+      <c r="B160" s="8"/>
     </row>
     <row r="161" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B161" s="4"/>
+      <c r="B161" s="8"/>
     </row>
     <row r="162" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B162" s="4"/>
+      <c r="B162" s="8"/>
     </row>
     <row r="163" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B163" s="4"/>
+      <c r="B163" s="8"/>
     </row>
     <row r="164" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B164" s="4"/>
+      <c r="B164" s="8"/>
     </row>
     <row r="165" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B165" s="4"/>
+      <c r="B165" s="8"/>
     </row>
     <row r="166" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B166" s="4"/>
+      <c r="B166" s="8"/>
     </row>
     <row r="167" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B167" s="4"/>
+      <c r="B167" s="8"/>
     </row>
     <row r="168" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B168" s="4"/>
+      <c r="B168" s="8"/>
     </row>
     <row r="169" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B169" s="4"/>
+      <c r="B169" s="8"/>
     </row>
     <row r="170" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B170" s="4"/>
+      <c r="B170" s="8"/>
     </row>
     <row r="171" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B171" s="4"/>
+      <c r="B171" s="8"/>
     </row>
     <row r="172" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B172" s="4"/>
+      <c r="B172" s="8"/>
     </row>
     <row r="173" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B173" s="4"/>
+      <c r="B173" s="8"/>
     </row>
     <row r="174" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B174" s="4"/>
+      <c r="B174" s="8"/>
     </row>
     <row r="175" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B175" s="4"/>
+      <c r="B175" s="8"/>
     </row>
     <row r="176" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B176" s="4"/>
+      <c r="B176" s="8"/>
     </row>
     <row r="177" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B177" s="4"/>
+      <c r="B177" s="8"/>
     </row>
     <row r="178" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B178" s="4"/>
+      <c r="B178" s="8"/>
     </row>
     <row r="179" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B179" s="4"/>
+      <c r="B179" s="8"/>
     </row>
     <row r="180" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B180" s="4"/>
+      <c r="B180" s="8"/>
     </row>
     <row r="181" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B181" s="4"/>
+      <c r="B181" s="8"/>
     </row>
     <row r="182" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B182" s="4"/>
+      <c r="B182" s="8"/>
     </row>
     <row r="183" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B183" s="4"/>
+      <c r="B183" s="8"/>
     </row>
     <row r="184" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B184" s="4"/>
+      <c r="B184" s="8"/>
     </row>
     <row r="185" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B185" s="4"/>
+      <c r="B185" s="8"/>
     </row>
     <row r="186" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B186" s="4"/>
+      <c r="B186" s="8"/>
     </row>
     <row r="187" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B187" s="4"/>
+      <c r="B187" s="8"/>
     </row>
     <row r="188" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B188" s="4"/>
+      <c r="B188" s="8"/>
     </row>
     <row r="189" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B189" s="4"/>
+      <c r="B189" s="8"/>
     </row>
     <row r="190" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B190" s="4"/>
+      <c r="B190" s="8"/>
     </row>
     <row r="191" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B191" s="4"/>
+      <c r="B191" s="8"/>
     </row>
     <row r="192" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B192" s="4"/>
+      <c r="B192" s="8"/>
     </row>
     <row r="193" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B193" s="4"/>
+      <c r="B193" s="8"/>
     </row>
     <row r="194" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B194" s="4"/>
+      <c r="B194" s="8"/>
     </row>
     <row r="195" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B195" s="4"/>
+      <c r="B195" s="8"/>
     </row>
     <row r="196" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B196" s="4"/>
+      <c r="B196" s="8"/>
     </row>
     <row r="197" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B197" s="4"/>
+      <c r="B197" s="8"/>
     </row>
     <row r="198" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B198" s="4"/>
+      <c r="B198" s="8"/>
     </row>
     <row r="199" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B199" s="4"/>
+      <c r="B199" s="8"/>
     </row>
     <row r="200" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B200" s="4"/>
+      <c r="B200" s="8"/>
     </row>
     <row r="201" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B201" s="4"/>
+      <c r="B201" s="8"/>
     </row>
     <row r="202" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B202" s="4"/>
+      <c r="B202" s="8"/>
     </row>
     <row r="203" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B203" s="4"/>
+      <c r="B203" s="8"/>
     </row>
     <row r="204" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B204" s="4"/>
+      <c r="B204" s="8"/>
     </row>
     <row r="205" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B205" s="4"/>
+      <c r="B205" s="8"/>
     </row>
     <row r="206" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B206" s="4"/>
+      <c r="B206" s="8"/>
     </row>
     <row r="207" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B207" s="4"/>
+      <c r="B207" s="8"/>
     </row>
     <row r="208" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B208" s="4"/>
+      <c r="B208" s="8"/>
     </row>
     <row r="209" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B209" s="4"/>
+      <c r="B209" s="8"/>
     </row>
     <row r="210" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B210" s="4"/>
+      <c r="B210" s="8"/>
     </row>
     <row r="211" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B211" s="4"/>
+      <c r="B211" s="8"/>
     </row>
     <row r="212" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B212" s="4"/>
+      <c r="B212" s="8"/>
     </row>
     <row r="213" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B213" s="4"/>
+      <c r="B213" s="8"/>
     </row>
     <row r="214" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B214" s="4"/>
+      <c r="B214" s="8"/>
     </row>
     <row r="215" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B215" s="4"/>
+      <c r="B215" s="8"/>
     </row>
     <row r="216" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B216" s="4"/>
+      <c r="B216" s="8"/>
     </row>
     <row r="217" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B217" s="4"/>
+      <c r="B217" s="8"/>
     </row>
     <row r="218" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B218" s="4"/>
+      <c r="B218" s="8"/>
     </row>
     <row r="219" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B219" s="4"/>
+      <c r="B219" s="8"/>
     </row>
     <row r="220" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B220" s="4"/>
+      <c r="B220" s="8"/>
     </row>
     <row r="221" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="222" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3461,6 +3520,7 @@
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="YKxeKJGY8Os762HkfL9qo0nuPTXQBAhOFoDd/A8/t1D5oEiNO7FqqXD0HoGFTa2wXhhvXzdX4RthrkI0lYgJ8Q==" saltValue="wfT1YPQlpsbC512iUVH8RQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <conditionalFormatting sqref="B2:B1000">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
       <formula>0</formula>

</xml_diff>